<commit_message>
Fixed compiler issues and refactored Asha's code to read subject details from excel sheet
</commit_message>
<xml_diff>
--- a/cis-util/data/subjects.xlsx
+++ b/cis-util/data/subjects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18680" windowHeight="5950"/>
   </bookViews>
   <sheets>
     <sheet name="subjects" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="44">
   <si>
     <t>ENGINEERING MATHEMATICS – III</t>
   </si>
   <si>
     <t>10 MAT 31</t>
-  </si>
-  <si>
-    <t>IA Marks</t>
-  </si>
-  <si>
-    <t>Exam Hrs</t>
-  </si>
-  <si>
-    <t>Hrs/Week</t>
   </si>
   <si>
     <t>A</t>
@@ -165,18 +156,6 @@
   </si>
   <si>
     <t>10MAT41</t>
-  </si>
-  <si>
-    <t>Total Hrs</t>
-  </si>
-  <si>
-    <t>Exam Marks</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Subject name</t>
   </si>
   <si>
     <t>10ESL36</t>
@@ -186,16 +165,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -244,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -254,7 +225,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -272,9 +242,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,34 +567,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>47</v>
+      <c r="F1" s="2">
+        <v>52</v>
+      </c>
+      <c r="G1" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>44</v>
+      <c r="A2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="2">
         <v>25</v>
@@ -646,11 +613,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="C3" s="2">
         <v>25</v>
@@ -669,11 +636,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="C4" s="2">
         <v>25</v>
@@ -692,11 +659,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>34</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="2">
         <v>25</v>
@@ -715,11 +682,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>35</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="2">
         <v>25</v>
@@ -738,11 +705,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="2">
         <v>25</v>
@@ -751,21 +718,21 @@
         <v>3</v>
       </c>
       <c r="E7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>40</v>
+      <c r="B8" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="2">
         <v>25</v>
@@ -784,11 +751,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>25</v>
@@ -797,35 +764,12 @@
         <v>3</v>
       </c>
       <c r="E9" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="G9" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="2">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2">
-        <v>52</v>
-      </c>
-      <c r="G10" s="2">
         <v>100</v>
       </c>
     </row>
@@ -839,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,181 +799,181 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>6</v>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F3" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="F4" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="F5" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8">
-        <v>5</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="E7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F7" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="8" t="s">
+      <c r="F8" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="8">
-        <v>6</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="7">
+        <v>8</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="8">
-        <v>7</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="10">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="8">
-        <v>8</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>6</v>
       </c>
     </row>
@@ -1064,30 +1008,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1095,10 +1039,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1106,10 +1050,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1117,10 +1061,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1128,10 +1072,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1139,10 +1083,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1150,10 +1094,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1161,10 +1105,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1195,30 +1139,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1226,10 +1170,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1237,10 +1181,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1248,10 +1192,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1259,10 +1203,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1270,10 +1214,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1281,10 +1225,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1292,10 +1236,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1326,30 +1270,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1357,10 +1301,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1368,10 +1312,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1379,10 +1323,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1390,10 +1334,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1401,10 +1345,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1412,10 +1356,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1423,10 +1367,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1457,30 +1401,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1488,10 +1432,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1499,10 +1443,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1510,10 +1454,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1521,10 +1465,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1532,10 +1476,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1543,10 +1487,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1554,10 +1498,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1588,30 +1532,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1619,10 +1563,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1630,10 +1574,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1641,10 +1585,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1652,10 +1596,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1663,10 +1607,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1674,10 +1618,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1685,10 +1629,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1719,30 +1663,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1750,10 +1694,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1761,10 +1705,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1772,10 +1716,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1783,10 +1727,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1794,10 +1738,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1805,10 +1749,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1816,10 +1760,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1850,30 +1794,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1881,10 +1825,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1892,10 +1836,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1903,10 +1847,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1914,10 +1858,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -1925,10 +1869,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1936,10 +1880,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1947,10 +1891,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9">
         <v>8</v>

</xml_diff>